<commit_message>
removed 1995, retrained and score
</commit_message>
<xml_diff>
--- a/Data_Gathering/Results_all.xlsx
+++ b/Data_Gathering/Results_all.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2104"/>
+  <dimension ref="A1:L2052"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -94841,2398 +94841,6 @@
         </is>
       </c>
     </row>
-    <row r="2053">
-      <c r="A2053" s="1" t="n">
-        <v>2051</v>
-      </c>
-      <c r="B2053" s="2" t="n">
-        <v>35063</v>
-      </c>
-      <c r="C2053" t="inlineStr">
-        <is>
-          <t>1,4,14,15,20,39</t>
-        </is>
-      </c>
-      <c r="D2053" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2053" t="n">
-        <v>4</v>
-      </c>
-      <c r="F2053" t="n">
-        <v>14</v>
-      </c>
-      <c r="G2053" t="n">
-        <v>15</v>
-      </c>
-      <c r="H2053" t="n">
-        <v>20</v>
-      </c>
-      <c r="I2053" t="n">
-        <v>39</v>
-      </c>
-      <c r="J2053" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="K2053" t="inlineStr">
-        <is>
-          <t>odd-even-even-odd-even-odd</t>
-        </is>
-      </c>
-      <c r="L2053" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2054">
-      <c r="A2054" s="1" t="n">
-        <v>2052</v>
-      </c>
-      <c r="B2054" s="2" t="n">
-        <v>35060</v>
-      </c>
-      <c r="C2054" t="inlineStr">
-        <is>
-          <t>5,7,12,16,23,30</t>
-        </is>
-      </c>
-      <c r="D2054" t="n">
-        <v>5</v>
-      </c>
-      <c r="E2054" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2054" t="n">
-        <v>12</v>
-      </c>
-      <c r="G2054" t="n">
-        <v>16</v>
-      </c>
-      <c r="H2054" t="n">
-        <v>23</v>
-      </c>
-      <c r="I2054" t="n">
-        <v>30</v>
-      </c>
-      <c r="J2054" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2054" t="inlineStr">
-        <is>
-          <t>odd-odd-even-even-odd-even</t>
-        </is>
-      </c>
-      <c r="L2054" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2055">
-      <c r="A2055" s="1" t="n">
-        <v>2053</v>
-      </c>
-      <c r="B2055" s="2" t="n">
-        <v>35056</v>
-      </c>
-      <c r="C2055" t="inlineStr">
-        <is>
-          <t>12,16,34,37,39,40</t>
-        </is>
-      </c>
-      <c r="D2055" t="n">
-        <v>12</v>
-      </c>
-      <c r="E2055" t="n">
-        <v>16</v>
-      </c>
-      <c r="F2055" t="n">
-        <v>34</v>
-      </c>
-      <c r="G2055" t="n">
-        <v>37</v>
-      </c>
-      <c r="H2055" t="n">
-        <v>39</v>
-      </c>
-      <c r="I2055" t="n">
-        <v>40</v>
-      </c>
-      <c r="J2055" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="K2055" t="inlineStr">
-        <is>
-          <t>even-even-even-odd-odd-even</t>
-        </is>
-      </c>
-      <c r="L2055" t="inlineStr">
-        <is>
-          <t>Even: 4, Odd: 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2056">
-      <c r="A2056" s="1" t="n">
-        <v>2054</v>
-      </c>
-      <c r="B2056" s="2" t="n">
-        <v>35053</v>
-      </c>
-      <c r="C2056" t="inlineStr">
-        <is>
-          <t>2,10,27,31,38,39</t>
-        </is>
-      </c>
-      <c r="D2056" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2056" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2056" t="n">
-        <v>27</v>
-      </c>
-      <c r="G2056" t="n">
-        <v>31</v>
-      </c>
-      <c r="H2056" t="n">
-        <v>38</v>
-      </c>
-      <c r="I2056" t="n">
-        <v>39</v>
-      </c>
-      <c r="J2056" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2056" t="inlineStr">
-        <is>
-          <t>even-even-odd-odd-even-odd</t>
-        </is>
-      </c>
-      <c r="L2056" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2057">
-      <c r="A2057" s="1" t="n">
-        <v>2055</v>
-      </c>
-      <c r="B2057" s="2" t="n">
-        <v>35049</v>
-      </c>
-      <c r="C2057" t="inlineStr">
-        <is>
-          <t>12,15,21,25,39,42</t>
-        </is>
-      </c>
-      <c r="D2057" t="n">
-        <v>12</v>
-      </c>
-      <c r="E2057" t="n">
-        <v>15</v>
-      </c>
-      <c r="F2057" t="n">
-        <v>21</v>
-      </c>
-      <c r="G2057" t="n">
-        <v>25</v>
-      </c>
-      <c r="H2057" t="n">
-        <v>39</v>
-      </c>
-      <c r="I2057" t="n">
-        <v>42</v>
-      </c>
-      <c r="J2057" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="K2057" t="inlineStr">
-        <is>
-          <t>even-odd-odd-odd-odd-even</t>
-        </is>
-      </c>
-      <c r="L2057" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2058">
-      <c r="A2058" s="1" t="n">
-        <v>2056</v>
-      </c>
-      <c r="B2058" s="2" t="n">
-        <v>35046</v>
-      </c>
-      <c r="C2058" t="inlineStr">
-        <is>
-          <t>2,4,11,16,23,31</t>
-        </is>
-      </c>
-      <c r="D2058" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2058" t="n">
-        <v>4</v>
-      </c>
-      <c r="F2058" t="n">
-        <v>11</v>
-      </c>
-      <c r="G2058" t="n">
-        <v>16</v>
-      </c>
-      <c r="H2058" t="n">
-        <v>23</v>
-      </c>
-      <c r="I2058" t="n">
-        <v>31</v>
-      </c>
-      <c r="J2058" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2058" t="inlineStr">
-        <is>
-          <t>even-even-odd-even-odd-odd</t>
-        </is>
-      </c>
-      <c r="L2058" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2059">
-      <c r="A2059" s="1" t="n">
-        <v>2057</v>
-      </c>
-      <c r="B2059" s="2" t="n">
-        <v>35042</v>
-      </c>
-      <c r="C2059" t="inlineStr">
-        <is>
-          <t>6,7,8,21,24,26</t>
-        </is>
-      </c>
-      <c r="D2059" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2059" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2059" t="n">
-        <v>8</v>
-      </c>
-      <c r="G2059" t="n">
-        <v>21</v>
-      </c>
-      <c r="H2059" t="n">
-        <v>24</v>
-      </c>
-      <c r="I2059" t="n">
-        <v>26</v>
-      </c>
-      <c r="J2059" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="K2059" t="inlineStr">
-        <is>
-          <t>even-odd-even-odd-even-even</t>
-        </is>
-      </c>
-      <c r="L2059" t="inlineStr">
-        <is>
-          <t>Even: 4, Odd: 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2060">
-      <c r="A2060" s="1" t="n">
-        <v>2058</v>
-      </c>
-      <c r="B2060" s="2" t="n">
-        <v>35039</v>
-      </c>
-      <c r="C2060" t="inlineStr">
-        <is>
-          <t>6,8,26,35,36,41</t>
-        </is>
-      </c>
-      <c r="D2060" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2060" t="n">
-        <v>8</v>
-      </c>
-      <c r="F2060" t="n">
-        <v>26</v>
-      </c>
-      <c r="G2060" t="n">
-        <v>35</v>
-      </c>
-      <c r="H2060" t="n">
-        <v>36</v>
-      </c>
-      <c r="I2060" t="n">
-        <v>41</v>
-      </c>
-      <c r="J2060" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2060" t="inlineStr">
-        <is>
-          <t>even-even-even-odd-even-odd</t>
-        </is>
-      </c>
-      <c r="L2060" t="inlineStr">
-        <is>
-          <t>Even: 4, Odd: 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2061">
-      <c r="A2061" s="1" t="n">
-        <v>2059</v>
-      </c>
-      <c r="B2061" s="2" t="n">
-        <v>35035</v>
-      </c>
-      <c r="C2061" t="inlineStr">
-        <is>
-          <t>7,8,11,15,18,22</t>
-        </is>
-      </c>
-      <c r="D2061" t="n">
-        <v>7</v>
-      </c>
-      <c r="E2061" t="n">
-        <v>8</v>
-      </c>
-      <c r="F2061" t="n">
-        <v>11</v>
-      </c>
-      <c r="G2061" t="n">
-        <v>15</v>
-      </c>
-      <c r="H2061" t="n">
-        <v>18</v>
-      </c>
-      <c r="I2061" t="n">
-        <v>22</v>
-      </c>
-      <c r="J2061" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="K2061" t="inlineStr">
-        <is>
-          <t>odd-even-odd-odd-even-even</t>
-        </is>
-      </c>
-      <c r="L2061" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2062">
-      <c r="A2062" s="1" t="n">
-        <v>2060</v>
-      </c>
-      <c r="B2062" s="2" t="n">
-        <v>35032</v>
-      </c>
-      <c r="C2062" t="inlineStr">
-        <is>
-          <t>2,17,22,25,26,39</t>
-        </is>
-      </c>
-      <c r="D2062" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2062" t="n">
-        <v>17</v>
-      </c>
-      <c r="F2062" t="n">
-        <v>22</v>
-      </c>
-      <c r="G2062" t="n">
-        <v>25</v>
-      </c>
-      <c r="H2062" t="n">
-        <v>26</v>
-      </c>
-      <c r="I2062" t="n">
-        <v>39</v>
-      </c>
-      <c r="J2062" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2062" t="inlineStr">
-        <is>
-          <t>even-odd-even-odd-even-odd</t>
-        </is>
-      </c>
-      <c r="L2062" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2063">
-      <c r="A2063" s="1" t="n">
-        <v>2061</v>
-      </c>
-      <c r="B2063" s="2" t="n">
-        <v>35028</v>
-      </c>
-      <c r="C2063" t="inlineStr">
-        <is>
-          <t>6,17,21,33,35,38</t>
-        </is>
-      </c>
-      <c r="D2063" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2063" t="n">
-        <v>17</v>
-      </c>
-      <c r="F2063" t="n">
-        <v>21</v>
-      </c>
-      <c r="G2063" t="n">
-        <v>33</v>
-      </c>
-      <c r="H2063" t="n">
-        <v>35</v>
-      </c>
-      <c r="I2063" t="n">
-        <v>38</v>
-      </c>
-      <c r="J2063" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="K2063" t="inlineStr">
-        <is>
-          <t>even-odd-odd-odd-odd-even</t>
-        </is>
-      </c>
-      <c r="L2063" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2064">
-      <c r="A2064" s="1" t="n">
-        <v>2062</v>
-      </c>
-      <c r="B2064" s="2" t="n">
-        <v>35025</v>
-      </c>
-      <c r="C2064" t="inlineStr">
-        <is>
-          <t>5,7,8,21,28,39</t>
-        </is>
-      </c>
-      <c r="D2064" t="n">
-        <v>5</v>
-      </c>
-      <c r="E2064" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2064" t="n">
-        <v>8</v>
-      </c>
-      <c r="G2064" t="n">
-        <v>21</v>
-      </c>
-      <c r="H2064" t="n">
-        <v>28</v>
-      </c>
-      <c r="I2064" t="n">
-        <v>39</v>
-      </c>
-      <c r="J2064" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2064" t="inlineStr">
-        <is>
-          <t>odd-odd-even-odd-even-odd</t>
-        </is>
-      </c>
-      <c r="L2064" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2065">
-      <c r="A2065" s="1" t="n">
-        <v>2063</v>
-      </c>
-      <c r="B2065" s="2" t="n">
-        <v>35021</v>
-      </c>
-      <c r="C2065" t="inlineStr">
-        <is>
-          <t>3,11,19,32,39,42</t>
-        </is>
-      </c>
-      <c r="D2065" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2065" t="n">
-        <v>11</v>
-      </c>
-      <c r="F2065" t="n">
-        <v>19</v>
-      </c>
-      <c r="G2065" t="n">
-        <v>32</v>
-      </c>
-      <c r="H2065" t="n">
-        <v>39</v>
-      </c>
-      <c r="I2065" t="n">
-        <v>42</v>
-      </c>
-      <c r="J2065" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="K2065" t="inlineStr">
-        <is>
-          <t>odd-odd-odd-even-odd-even</t>
-        </is>
-      </c>
-      <c r="L2065" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2066">
-      <c r="A2066" s="1" t="n">
-        <v>2064</v>
-      </c>
-      <c r="B2066" s="2" t="n">
-        <v>35018</v>
-      </c>
-      <c r="C2066" t="inlineStr">
-        <is>
-          <t>4,6,7,14,15,36</t>
-        </is>
-      </c>
-      <c r="D2066" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2066" t="n">
-        <v>6</v>
-      </c>
-      <c r="F2066" t="n">
-        <v>7</v>
-      </c>
-      <c r="G2066" t="n">
-        <v>14</v>
-      </c>
-      <c r="H2066" t="n">
-        <v>15</v>
-      </c>
-      <c r="I2066" t="n">
-        <v>36</v>
-      </c>
-      <c r="J2066" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2066" t="inlineStr">
-        <is>
-          <t>even-even-odd-even-odd-even</t>
-        </is>
-      </c>
-      <c r="L2066" t="inlineStr">
-        <is>
-          <t>Even: 4, Odd: 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2067">
-      <c r="A2067" s="1" t="n">
-        <v>2065</v>
-      </c>
-      <c r="B2067" s="2" t="n">
-        <v>35014</v>
-      </c>
-      <c r="C2067" t="inlineStr">
-        <is>
-          <t>3,20,31,33,39,42</t>
-        </is>
-      </c>
-      <c r="D2067" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2067" t="n">
-        <v>20</v>
-      </c>
-      <c r="F2067" t="n">
-        <v>31</v>
-      </c>
-      <c r="G2067" t="n">
-        <v>33</v>
-      </c>
-      <c r="H2067" t="n">
-        <v>39</v>
-      </c>
-      <c r="I2067" t="n">
-        <v>42</v>
-      </c>
-      <c r="J2067" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="K2067" t="inlineStr">
-        <is>
-          <t>odd-even-odd-odd-odd-even</t>
-        </is>
-      </c>
-      <c r="L2067" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2068">
-      <c r="A2068" s="1" t="n">
-        <v>2066</v>
-      </c>
-      <c r="B2068" s="2" t="n">
-        <v>35011</v>
-      </c>
-      <c r="C2068" t="inlineStr">
-        <is>
-          <t>1,3,11,23,31,34</t>
-        </is>
-      </c>
-      <c r="D2068" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2068" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2068" t="n">
-        <v>11</v>
-      </c>
-      <c r="G2068" t="n">
-        <v>23</v>
-      </c>
-      <c r="H2068" t="n">
-        <v>31</v>
-      </c>
-      <c r="I2068" t="n">
-        <v>34</v>
-      </c>
-      <c r="J2068" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2068" t="inlineStr">
-        <is>
-          <t>odd-odd-odd-odd-odd-even</t>
-        </is>
-      </c>
-      <c r="L2068" t="inlineStr">
-        <is>
-          <t>Even: 1, Odd: 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="2069">
-      <c r="A2069" s="1" t="n">
-        <v>2067</v>
-      </c>
-      <c r="B2069" s="2" t="n">
-        <v>35004</v>
-      </c>
-      <c r="C2069" t="inlineStr">
-        <is>
-          <t>2,13,27,30,39,42</t>
-        </is>
-      </c>
-      <c r="D2069" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2069" t="n">
-        <v>13</v>
-      </c>
-      <c r="F2069" t="n">
-        <v>27</v>
-      </c>
-      <c r="G2069" t="n">
-        <v>30</v>
-      </c>
-      <c r="H2069" t="n">
-        <v>39</v>
-      </c>
-      <c r="I2069" t="n">
-        <v>42</v>
-      </c>
-      <c r="J2069" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2069" t="inlineStr">
-        <is>
-          <t>even-odd-odd-even-odd-even</t>
-        </is>
-      </c>
-      <c r="L2069" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2070">
-      <c r="A2070" s="1" t="n">
-        <v>2068</v>
-      </c>
-      <c r="B2070" s="2" t="n">
-        <v>34997</v>
-      </c>
-      <c r="C2070" t="inlineStr">
-        <is>
-          <t>10,12,18,20,35,39</t>
-        </is>
-      </c>
-      <c r="D2070" t="n">
-        <v>10</v>
-      </c>
-      <c r="E2070" t="n">
-        <v>12</v>
-      </c>
-      <c r="F2070" t="n">
-        <v>18</v>
-      </c>
-      <c r="G2070" t="n">
-        <v>20</v>
-      </c>
-      <c r="H2070" t="n">
-        <v>35</v>
-      </c>
-      <c r="I2070" t="n">
-        <v>39</v>
-      </c>
-      <c r="J2070" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2070" t="inlineStr">
-        <is>
-          <t>even-even-even-even-odd-odd</t>
-        </is>
-      </c>
-      <c r="L2070" t="inlineStr">
-        <is>
-          <t>Even: 4, Odd: 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2071">
-      <c r="A2071" s="1" t="n">
-        <v>2069</v>
-      </c>
-      <c r="B2071" s="2" t="n">
-        <v>34990</v>
-      </c>
-      <c r="C2071" t="inlineStr">
-        <is>
-          <t>6,10,14,34,39,42</t>
-        </is>
-      </c>
-      <c r="D2071" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2071" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2071" t="n">
-        <v>14</v>
-      </c>
-      <c r="G2071" t="n">
-        <v>34</v>
-      </c>
-      <c r="H2071" t="n">
-        <v>39</v>
-      </c>
-      <c r="I2071" t="n">
-        <v>42</v>
-      </c>
-      <c r="J2071" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2071" t="inlineStr">
-        <is>
-          <t>even-even-even-even-odd-even</t>
-        </is>
-      </c>
-      <c r="L2071" t="inlineStr">
-        <is>
-          <t>Even: 5, Odd: 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="2072">
-      <c r="A2072" s="1" t="n">
-        <v>2070</v>
-      </c>
-      <c r="B2072" s="2" t="n">
-        <v>34983</v>
-      </c>
-      <c r="C2072" t="inlineStr">
-        <is>
-          <t>9,14,20,22,29,35</t>
-        </is>
-      </c>
-      <c r="D2072" t="n">
-        <v>9</v>
-      </c>
-      <c r="E2072" t="n">
-        <v>14</v>
-      </c>
-      <c r="F2072" t="n">
-        <v>20</v>
-      </c>
-      <c r="G2072" t="n">
-        <v>22</v>
-      </c>
-      <c r="H2072" t="n">
-        <v>29</v>
-      </c>
-      <c r="I2072" t="n">
-        <v>35</v>
-      </c>
-      <c r="J2072" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2072" t="inlineStr">
-        <is>
-          <t>odd-even-even-even-odd-odd</t>
-        </is>
-      </c>
-      <c r="L2072" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2073">
-      <c r="A2073" s="1" t="n">
-        <v>2071</v>
-      </c>
-      <c r="B2073" s="2" t="n">
-        <v>34976</v>
-      </c>
-      <c r="C2073" t="inlineStr">
-        <is>
-          <t>7,10,17,24,26,36</t>
-        </is>
-      </c>
-      <c r="D2073" t="n">
-        <v>7</v>
-      </c>
-      <c r="E2073" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2073" t="n">
-        <v>17</v>
-      </c>
-      <c r="G2073" t="n">
-        <v>24</v>
-      </c>
-      <c r="H2073" t="n">
-        <v>26</v>
-      </c>
-      <c r="I2073" t="n">
-        <v>36</v>
-      </c>
-      <c r="J2073" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2073" t="inlineStr">
-        <is>
-          <t>odd-even-odd-even-even-even</t>
-        </is>
-      </c>
-      <c r="L2073" t="inlineStr">
-        <is>
-          <t>Even: 4, Odd: 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2074">
-      <c r="A2074" s="1" t="n">
-        <v>2072</v>
-      </c>
-      <c r="B2074" s="2" t="n">
-        <v>34969</v>
-      </c>
-      <c r="C2074" t="inlineStr">
-        <is>
-          <t>5,18,20,24,27,35</t>
-        </is>
-      </c>
-      <c r="D2074" t="n">
-        <v>5</v>
-      </c>
-      <c r="E2074" t="n">
-        <v>18</v>
-      </c>
-      <c r="F2074" t="n">
-        <v>20</v>
-      </c>
-      <c r="G2074" t="n">
-        <v>24</v>
-      </c>
-      <c r="H2074" t="n">
-        <v>27</v>
-      </c>
-      <c r="I2074" t="n">
-        <v>35</v>
-      </c>
-      <c r="J2074" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2074" t="inlineStr">
-        <is>
-          <t>odd-even-even-even-odd-odd</t>
-        </is>
-      </c>
-      <c r="L2074" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2075">
-      <c r="A2075" s="1" t="n">
-        <v>2073</v>
-      </c>
-      <c r="B2075" s="2" t="n">
-        <v>34962</v>
-      </c>
-      <c r="C2075" t="inlineStr">
-        <is>
-          <t>6,12,19,34,41,42</t>
-        </is>
-      </c>
-      <c r="D2075" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2075" t="n">
-        <v>12</v>
-      </c>
-      <c r="F2075" t="n">
-        <v>19</v>
-      </c>
-      <c r="G2075" t="n">
-        <v>34</v>
-      </c>
-      <c r="H2075" t="n">
-        <v>41</v>
-      </c>
-      <c r="I2075" t="n">
-        <v>42</v>
-      </c>
-      <c r="J2075" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2075" t="inlineStr">
-        <is>
-          <t>even-even-odd-even-odd-even</t>
-        </is>
-      </c>
-      <c r="L2075" t="inlineStr">
-        <is>
-          <t>Even: 4, Odd: 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2076">
-      <c r="A2076" s="1" t="n">
-        <v>2074</v>
-      </c>
-      <c r="B2076" s="2" t="n">
-        <v>34955</v>
-      </c>
-      <c r="C2076" t="inlineStr">
-        <is>
-          <t>4,8,9,27,28,39</t>
-        </is>
-      </c>
-      <c r="D2076" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2076" t="n">
-        <v>8</v>
-      </c>
-      <c r="F2076" t="n">
-        <v>9</v>
-      </c>
-      <c r="G2076" t="n">
-        <v>27</v>
-      </c>
-      <c r="H2076" t="n">
-        <v>28</v>
-      </c>
-      <c r="I2076" t="n">
-        <v>39</v>
-      </c>
-      <c r="J2076" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2076" t="inlineStr">
-        <is>
-          <t>even-even-odd-odd-even-odd</t>
-        </is>
-      </c>
-      <c r="L2076" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2077">
-      <c r="A2077" s="1" t="n">
-        <v>2075</v>
-      </c>
-      <c r="B2077" s="2" t="n">
-        <v>34948</v>
-      </c>
-      <c r="C2077" t="inlineStr">
-        <is>
-          <t>16,18,23,31,38,41</t>
-        </is>
-      </c>
-      <c r="D2077" t="n">
-        <v>16</v>
-      </c>
-      <c r="E2077" t="n">
-        <v>18</v>
-      </c>
-      <c r="F2077" t="n">
-        <v>23</v>
-      </c>
-      <c r="G2077" t="n">
-        <v>31</v>
-      </c>
-      <c r="H2077" t="n">
-        <v>38</v>
-      </c>
-      <c r="I2077" t="n">
-        <v>41</v>
-      </c>
-      <c r="J2077" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2077" t="inlineStr">
-        <is>
-          <t>even-even-odd-odd-even-odd</t>
-        </is>
-      </c>
-      <c r="L2077" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2078">
-      <c r="A2078" s="1" t="n">
-        <v>2076</v>
-      </c>
-      <c r="B2078" s="2" t="n">
-        <v>34941</v>
-      </c>
-      <c r="C2078" t="inlineStr">
-        <is>
-          <t>2,3,9,21,33,36</t>
-        </is>
-      </c>
-      <c r="D2078" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2078" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2078" t="n">
-        <v>9</v>
-      </c>
-      <c r="G2078" t="n">
-        <v>21</v>
-      </c>
-      <c r="H2078" t="n">
-        <v>33</v>
-      </c>
-      <c r="I2078" t="n">
-        <v>36</v>
-      </c>
-      <c r="J2078" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2078" t="inlineStr">
-        <is>
-          <t>even-odd-odd-odd-odd-even</t>
-        </is>
-      </c>
-      <c r="L2078" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2079">
-      <c r="A2079" s="1" t="n">
-        <v>2077</v>
-      </c>
-      <c r="B2079" s="2" t="n">
-        <v>34934</v>
-      </c>
-      <c r="C2079" t="inlineStr">
-        <is>
-          <t>4,17,24,25,32,38</t>
-        </is>
-      </c>
-      <c r="D2079" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2079" t="n">
-        <v>17</v>
-      </c>
-      <c r="F2079" t="n">
-        <v>24</v>
-      </c>
-      <c r="G2079" t="n">
-        <v>25</v>
-      </c>
-      <c r="H2079" t="n">
-        <v>32</v>
-      </c>
-      <c r="I2079" t="n">
-        <v>38</v>
-      </c>
-      <c r="J2079" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2079" t="inlineStr">
-        <is>
-          <t>even-odd-even-odd-even-even</t>
-        </is>
-      </c>
-      <c r="L2079" t="inlineStr">
-        <is>
-          <t>Even: 4, Odd: 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2080">
-      <c r="A2080" s="1" t="n">
-        <v>2078</v>
-      </c>
-      <c r="B2080" s="2" t="n">
-        <v>34927</v>
-      </c>
-      <c r="C2080" t="inlineStr">
-        <is>
-          <t>3,9,10,14,26,41</t>
-        </is>
-      </c>
-      <c r="D2080" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2080" t="n">
-        <v>9</v>
-      </c>
-      <c r="F2080" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2080" t="n">
-        <v>14</v>
-      </c>
-      <c r="H2080" t="n">
-        <v>26</v>
-      </c>
-      <c r="I2080" t="n">
-        <v>41</v>
-      </c>
-      <c r="J2080" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2080" t="inlineStr">
-        <is>
-          <t>odd-odd-even-even-even-odd</t>
-        </is>
-      </c>
-      <c r="L2080" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2081">
-      <c r="A2081" s="1" t="n">
-        <v>2079</v>
-      </c>
-      <c r="B2081" s="2" t="n">
-        <v>34920</v>
-      </c>
-      <c r="C2081" t="inlineStr">
-        <is>
-          <t>3,8,17,23,29,37</t>
-        </is>
-      </c>
-      <c r="D2081" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2081" t="n">
-        <v>8</v>
-      </c>
-      <c r="F2081" t="n">
-        <v>17</v>
-      </c>
-      <c r="G2081" t="n">
-        <v>23</v>
-      </c>
-      <c r="H2081" t="n">
-        <v>29</v>
-      </c>
-      <c r="I2081" t="n">
-        <v>37</v>
-      </c>
-      <c r="J2081" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2081" t="inlineStr">
-        <is>
-          <t>odd-even-odd-odd-odd-odd</t>
-        </is>
-      </c>
-      <c r="L2081" t="inlineStr">
-        <is>
-          <t>Even: 1, Odd: 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="2082">
-      <c r="A2082" s="1" t="n">
-        <v>2080</v>
-      </c>
-      <c r="B2082" s="2" t="n">
-        <v>34913</v>
-      </c>
-      <c r="C2082" t="inlineStr">
-        <is>
-          <t>2,7,16,19,23,30</t>
-        </is>
-      </c>
-      <c r="D2082" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2082" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2082" t="n">
-        <v>16</v>
-      </c>
-      <c r="G2082" t="n">
-        <v>19</v>
-      </c>
-      <c r="H2082" t="n">
-        <v>23</v>
-      </c>
-      <c r="I2082" t="n">
-        <v>30</v>
-      </c>
-      <c r="J2082" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2082" t="inlineStr">
-        <is>
-          <t>even-odd-even-odd-odd-even</t>
-        </is>
-      </c>
-      <c r="L2082" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2083">
-      <c r="A2083" s="1" t="n">
-        <v>2081</v>
-      </c>
-      <c r="B2083" s="2" t="n">
-        <v>34906</v>
-      </c>
-      <c r="C2083" t="inlineStr">
-        <is>
-          <t>12,13,15,17,19,33</t>
-        </is>
-      </c>
-      <c r="D2083" t="n">
-        <v>12</v>
-      </c>
-      <c r="E2083" t="n">
-        <v>13</v>
-      </c>
-      <c r="F2083" t="n">
-        <v>15</v>
-      </c>
-      <c r="G2083" t="n">
-        <v>17</v>
-      </c>
-      <c r="H2083" t="n">
-        <v>19</v>
-      </c>
-      <c r="I2083" t="n">
-        <v>33</v>
-      </c>
-      <c r="J2083" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2083" t="inlineStr">
-        <is>
-          <t>even-odd-odd-odd-odd-odd</t>
-        </is>
-      </c>
-      <c r="L2083" t="inlineStr">
-        <is>
-          <t>Even: 1, Odd: 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="2084">
-      <c r="A2084" s="1" t="n">
-        <v>2082</v>
-      </c>
-      <c r="B2084" s="2" t="n">
-        <v>34899</v>
-      </c>
-      <c r="C2084" t="inlineStr">
-        <is>
-          <t>9,17,21,27,32,42</t>
-        </is>
-      </c>
-      <c r="D2084" t="n">
-        <v>9</v>
-      </c>
-      <c r="E2084" t="n">
-        <v>17</v>
-      </c>
-      <c r="F2084" t="n">
-        <v>21</v>
-      </c>
-      <c r="G2084" t="n">
-        <v>27</v>
-      </c>
-      <c r="H2084" t="n">
-        <v>32</v>
-      </c>
-      <c r="I2084" t="n">
-        <v>42</v>
-      </c>
-      <c r="J2084" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2084" t="inlineStr">
-        <is>
-          <t>odd-odd-odd-odd-even-even</t>
-        </is>
-      </c>
-      <c r="L2084" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2085">
-      <c r="A2085" s="1" t="n">
-        <v>2083</v>
-      </c>
-      <c r="B2085" s="2" t="n">
-        <v>34892</v>
-      </c>
-      <c r="C2085" t="inlineStr">
-        <is>
-          <t>3,5,7,12,18,25</t>
-        </is>
-      </c>
-      <c r="D2085" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2085" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2085" t="n">
-        <v>7</v>
-      </c>
-      <c r="G2085" t="n">
-        <v>12</v>
-      </c>
-      <c r="H2085" t="n">
-        <v>18</v>
-      </c>
-      <c r="I2085" t="n">
-        <v>25</v>
-      </c>
-      <c r="J2085" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2085" t="inlineStr">
-        <is>
-          <t>odd-odd-odd-even-even-odd</t>
-        </is>
-      </c>
-      <c r="L2085" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2086">
-      <c r="A2086" s="1" t="n">
-        <v>2084</v>
-      </c>
-      <c r="B2086" s="2" t="n">
-        <v>34885</v>
-      </c>
-      <c r="C2086" t="inlineStr">
-        <is>
-          <t>8,10,22,34,35,38</t>
-        </is>
-      </c>
-      <c r="D2086" t="n">
-        <v>8</v>
-      </c>
-      <c r="E2086" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2086" t="n">
-        <v>22</v>
-      </c>
-      <c r="G2086" t="n">
-        <v>34</v>
-      </c>
-      <c r="H2086" t="n">
-        <v>35</v>
-      </c>
-      <c r="I2086" t="n">
-        <v>38</v>
-      </c>
-      <c r="J2086" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2086" t="inlineStr">
-        <is>
-          <t>even-even-even-even-odd-even</t>
-        </is>
-      </c>
-      <c r="L2086" t="inlineStr">
-        <is>
-          <t>Even: 5, Odd: 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="2087">
-      <c r="A2087" s="1" t="n">
-        <v>2085</v>
-      </c>
-      <c r="B2087" s="2" t="n">
-        <v>34878</v>
-      </c>
-      <c r="C2087" t="inlineStr">
-        <is>
-          <t>1,7,9,19,28,37</t>
-        </is>
-      </c>
-      <c r="D2087" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2087" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2087" t="n">
-        <v>9</v>
-      </c>
-      <c r="G2087" t="n">
-        <v>19</v>
-      </c>
-      <c r="H2087" t="n">
-        <v>28</v>
-      </c>
-      <c r="I2087" t="n">
-        <v>37</v>
-      </c>
-      <c r="J2087" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2087" t="inlineStr">
-        <is>
-          <t>odd-odd-odd-odd-even-odd</t>
-        </is>
-      </c>
-      <c r="L2087" t="inlineStr">
-        <is>
-          <t>Even: 1, Odd: 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="2088">
-      <c r="A2088" s="1" t="n">
-        <v>2086</v>
-      </c>
-      <c r="B2088" s="2" t="n">
-        <v>34871</v>
-      </c>
-      <c r="C2088" t="inlineStr">
-        <is>
-          <t>13,20,23,28,29,42</t>
-        </is>
-      </c>
-      <c r="D2088" t="n">
-        <v>13</v>
-      </c>
-      <c r="E2088" t="n">
-        <v>20</v>
-      </c>
-      <c r="F2088" t="n">
-        <v>23</v>
-      </c>
-      <c r="G2088" t="n">
-        <v>28</v>
-      </c>
-      <c r="H2088" t="n">
-        <v>29</v>
-      </c>
-      <c r="I2088" t="n">
-        <v>42</v>
-      </c>
-      <c r="J2088" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2088" t="inlineStr">
-        <is>
-          <t>odd-even-odd-even-odd-even</t>
-        </is>
-      </c>
-      <c r="L2088" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2089">
-      <c r="A2089" s="1" t="n">
-        <v>2087</v>
-      </c>
-      <c r="B2089" s="2" t="n">
-        <v>34864</v>
-      </c>
-      <c r="C2089" t="inlineStr">
-        <is>
-          <t>5,12,13,30,31,35</t>
-        </is>
-      </c>
-      <c r="D2089" t="n">
-        <v>5</v>
-      </c>
-      <c r="E2089" t="n">
-        <v>12</v>
-      </c>
-      <c r="F2089" t="n">
-        <v>13</v>
-      </c>
-      <c r="G2089" t="n">
-        <v>30</v>
-      </c>
-      <c r="H2089" t="n">
-        <v>31</v>
-      </c>
-      <c r="I2089" t="n">
-        <v>35</v>
-      </c>
-      <c r="J2089" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2089" t="inlineStr">
-        <is>
-          <t>odd-even-odd-even-odd-odd</t>
-        </is>
-      </c>
-      <c r="L2089" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2090">
-      <c r="A2090" s="1" t="n">
-        <v>2088</v>
-      </c>
-      <c r="B2090" s="2" t="n">
-        <v>34860</v>
-      </c>
-      <c r="C2090" t="inlineStr">
-        <is>
-          <t>1,3,13,21,36,40</t>
-        </is>
-      </c>
-      <c r="D2090" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2090" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2090" t="n">
-        <v>13</v>
-      </c>
-      <c r="G2090" t="n">
-        <v>21</v>
-      </c>
-      <c r="H2090" t="n">
-        <v>36</v>
-      </c>
-      <c r="I2090" t="n">
-        <v>40</v>
-      </c>
-      <c r="J2090" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="K2090" t="inlineStr">
-        <is>
-          <t>odd-odd-odd-odd-even-even</t>
-        </is>
-      </c>
-      <c r="L2090" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2091">
-      <c r="A2091" s="1" t="n">
-        <v>2089</v>
-      </c>
-      <c r="B2091" s="2" t="n">
-        <v>34857</v>
-      </c>
-      <c r="C2091" t="inlineStr">
-        <is>
-          <t>6,7,11,15,18,31</t>
-        </is>
-      </c>
-      <c r="D2091" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2091" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2091" t="n">
-        <v>11</v>
-      </c>
-      <c r="G2091" t="n">
-        <v>15</v>
-      </c>
-      <c r="H2091" t="n">
-        <v>18</v>
-      </c>
-      <c r="I2091" t="n">
-        <v>31</v>
-      </c>
-      <c r="J2091" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2091" t="inlineStr">
-        <is>
-          <t>even-odd-odd-odd-even-odd</t>
-        </is>
-      </c>
-      <c r="L2091" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2092">
-      <c r="A2092" s="1" t="n">
-        <v>2090</v>
-      </c>
-      <c r="B2092" s="2" t="n">
-        <v>34850</v>
-      </c>
-      <c r="C2092" t="inlineStr">
-        <is>
-          <t>1,9,10,15,36,39</t>
-        </is>
-      </c>
-      <c r="D2092" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2092" t="n">
-        <v>9</v>
-      </c>
-      <c r="F2092" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2092" t="n">
-        <v>15</v>
-      </c>
-      <c r="H2092" t="n">
-        <v>36</v>
-      </c>
-      <c r="I2092" t="n">
-        <v>39</v>
-      </c>
-      <c r="J2092" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2092" t="inlineStr">
-        <is>
-          <t>odd-odd-even-odd-even-odd</t>
-        </is>
-      </c>
-      <c r="L2092" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2093">
-      <c r="A2093" s="1" t="n">
-        <v>2091</v>
-      </c>
-      <c r="B2093" s="2" t="n">
-        <v>34843</v>
-      </c>
-      <c r="C2093" t="inlineStr">
-        <is>
-          <t>16,21,22,28,29,33</t>
-        </is>
-      </c>
-      <c r="D2093" t="n">
-        <v>16</v>
-      </c>
-      <c r="E2093" t="n">
-        <v>21</v>
-      </c>
-      <c r="F2093" t="n">
-        <v>22</v>
-      </c>
-      <c r="G2093" t="n">
-        <v>28</v>
-      </c>
-      <c r="H2093" t="n">
-        <v>29</v>
-      </c>
-      <c r="I2093" t="n">
-        <v>33</v>
-      </c>
-      <c r="J2093" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2093" t="inlineStr">
-        <is>
-          <t>even-odd-even-even-odd-odd</t>
-        </is>
-      </c>
-      <c r="L2093" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2094">
-      <c r="A2094" s="1" t="n">
-        <v>2092</v>
-      </c>
-      <c r="B2094" s="2" t="n">
-        <v>34836</v>
-      </c>
-      <c r="C2094" t="inlineStr">
-        <is>
-          <t>10,20,30,32,34,42</t>
-        </is>
-      </c>
-      <c r="D2094" t="n">
-        <v>10</v>
-      </c>
-      <c r="E2094" t="n">
-        <v>20</v>
-      </c>
-      <c r="F2094" t="n">
-        <v>30</v>
-      </c>
-      <c r="G2094" t="n">
-        <v>32</v>
-      </c>
-      <c r="H2094" t="n">
-        <v>34</v>
-      </c>
-      <c r="I2094" t="n">
-        <v>42</v>
-      </c>
-      <c r="J2094" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2094" t="inlineStr">
-        <is>
-          <t>even-even-even-even-even-even</t>
-        </is>
-      </c>
-      <c r="L2094" t="inlineStr">
-        <is>
-          <t>Even: 6, Odd: 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="2095">
-      <c r="A2095" s="1" t="n">
-        <v>2093</v>
-      </c>
-      <c r="B2095" s="2" t="n">
-        <v>34829</v>
-      </c>
-      <c r="C2095" t="inlineStr">
-        <is>
-          <t>8,9,10,25,28,33</t>
-        </is>
-      </c>
-      <c r="D2095" t="n">
-        <v>8</v>
-      </c>
-      <c r="E2095" t="n">
-        <v>9</v>
-      </c>
-      <c r="F2095" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2095" t="n">
-        <v>25</v>
-      </c>
-      <c r="H2095" t="n">
-        <v>28</v>
-      </c>
-      <c r="I2095" t="n">
-        <v>33</v>
-      </c>
-      <c r="J2095" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2095" t="inlineStr">
-        <is>
-          <t>even-odd-even-odd-even-odd</t>
-        </is>
-      </c>
-      <c r="L2095" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2096">
-      <c r="A2096" s="1" t="n">
-        <v>2094</v>
-      </c>
-      <c r="B2096" s="2" t="n">
-        <v>34822</v>
-      </c>
-      <c r="C2096" t="inlineStr">
-        <is>
-          <t>1,11,32,33,39,41</t>
-        </is>
-      </c>
-      <c r="D2096" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2096" t="n">
-        <v>11</v>
-      </c>
-      <c r="F2096" t="n">
-        <v>32</v>
-      </c>
-      <c r="G2096" t="n">
-        <v>33</v>
-      </c>
-      <c r="H2096" t="n">
-        <v>39</v>
-      </c>
-      <c r="I2096" t="n">
-        <v>41</v>
-      </c>
-      <c r="J2096" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2096" t="inlineStr">
-        <is>
-          <t>odd-odd-even-odd-odd-odd</t>
-        </is>
-      </c>
-      <c r="L2096" t="inlineStr">
-        <is>
-          <t>Even: 1, Odd: 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="2097">
-      <c r="A2097" s="1" t="n">
-        <v>2095</v>
-      </c>
-      <c r="B2097" s="2" t="n">
-        <v>34815</v>
-      </c>
-      <c r="C2097" t="inlineStr">
-        <is>
-          <t>1,14,15,27,32,40</t>
-        </is>
-      </c>
-      <c r="D2097" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2097" t="n">
-        <v>14</v>
-      </c>
-      <c r="F2097" t="n">
-        <v>15</v>
-      </c>
-      <c r="G2097" t="n">
-        <v>27</v>
-      </c>
-      <c r="H2097" t="n">
-        <v>32</v>
-      </c>
-      <c r="I2097" t="n">
-        <v>40</v>
-      </c>
-      <c r="J2097" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2097" t="inlineStr">
-        <is>
-          <t>odd-even-odd-odd-even-even</t>
-        </is>
-      </c>
-      <c r="L2097" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2098">
-      <c r="A2098" s="1" t="n">
-        <v>2096</v>
-      </c>
-      <c r="B2098" s="2" t="n">
-        <v>34808</v>
-      </c>
-      <c r="C2098" t="inlineStr">
-        <is>
-          <t>6,25,26,29,35,40</t>
-        </is>
-      </c>
-      <c r="D2098" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2098" t="n">
-        <v>25</v>
-      </c>
-      <c r="F2098" t="n">
-        <v>26</v>
-      </c>
-      <c r="G2098" t="n">
-        <v>29</v>
-      </c>
-      <c r="H2098" t="n">
-        <v>35</v>
-      </c>
-      <c r="I2098" t="n">
-        <v>40</v>
-      </c>
-      <c r="J2098" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2098" t="inlineStr">
-        <is>
-          <t>even-odd-even-odd-odd-even</t>
-        </is>
-      </c>
-      <c r="L2098" t="inlineStr">
-        <is>
-          <t>Even: 3, Odd: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2099">
-      <c r="A2099" s="1" t="n">
-        <v>2097</v>
-      </c>
-      <c r="B2099" s="2" t="n">
-        <v>34801</v>
-      </c>
-      <c r="C2099" t="inlineStr">
-        <is>
-          <t>1,4,18,25,32,40</t>
-        </is>
-      </c>
-      <c r="D2099" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2099" t="n">
-        <v>4</v>
-      </c>
-      <c r="F2099" t="n">
-        <v>18</v>
-      </c>
-      <c r="G2099" t="n">
-        <v>25</v>
-      </c>
-      <c r="H2099" t="n">
-        <v>32</v>
-      </c>
-      <c r="I2099" t="n">
-        <v>40</v>
-      </c>
-      <c r="J2099" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2099" t="inlineStr">
-        <is>
-          <t>odd-even-even-odd-even-even</t>
-        </is>
-      </c>
-      <c r="L2099" t="inlineStr">
-        <is>
-          <t>Even: 4, Odd: 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2100">
-      <c r="A2100" s="1" t="n">
-        <v>2098</v>
-      </c>
-      <c r="B2100" s="2" t="n">
-        <v>34794</v>
-      </c>
-      <c r="C2100" t="inlineStr">
-        <is>
-          <t>2,20,28,37,41,42</t>
-        </is>
-      </c>
-      <c r="D2100" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2100" t="n">
-        <v>20</v>
-      </c>
-      <c r="F2100" t="n">
-        <v>28</v>
-      </c>
-      <c r="G2100" t="n">
-        <v>37</v>
-      </c>
-      <c r="H2100" t="n">
-        <v>41</v>
-      </c>
-      <c r="I2100" t="n">
-        <v>42</v>
-      </c>
-      <c r="J2100" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2100" t="inlineStr">
-        <is>
-          <t>even-even-even-odd-odd-even</t>
-        </is>
-      </c>
-      <c r="L2100" t="inlineStr">
-        <is>
-          <t>Even: 4, Odd: 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2101">
-      <c r="A2101" s="1" t="n">
-        <v>2099</v>
-      </c>
-      <c r="B2101" s="2" t="n">
-        <v>34787</v>
-      </c>
-      <c r="C2101" t="inlineStr">
-        <is>
-          <t>1,9,25,26,37,40</t>
-        </is>
-      </c>
-      <c r="D2101" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2101" t="n">
-        <v>9</v>
-      </c>
-      <c r="F2101" t="n">
-        <v>25</v>
-      </c>
-      <c r="G2101" t="n">
-        <v>26</v>
-      </c>
-      <c r="H2101" t="n">
-        <v>37</v>
-      </c>
-      <c r="I2101" t="n">
-        <v>40</v>
-      </c>
-      <c r="J2101" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2101" t="inlineStr">
-        <is>
-          <t>odd-odd-odd-even-odd-even</t>
-        </is>
-      </c>
-      <c r="L2101" t="inlineStr">
-        <is>
-          <t>Even: 2, Odd: 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2102">
-      <c r="A2102" s="1" t="n">
-        <v>2100</v>
-      </c>
-      <c r="B2102" s="2" t="n">
-        <v>34780</v>
-      </c>
-      <c r="C2102" t="inlineStr">
-        <is>
-          <t>5,12,14,22,30,35</t>
-        </is>
-      </c>
-      <c r="D2102" t="n">
-        <v>5</v>
-      </c>
-      <c r="E2102" t="n">
-        <v>12</v>
-      </c>
-      <c r="F2102" t="n">
-        <v>14</v>
-      </c>
-      <c r="G2102" t="n">
-        <v>22</v>
-      </c>
-      <c r="H2102" t="n">
-        <v>30</v>
-      </c>
-      <c r="I2102" t="n">
-        <v>35</v>
-      </c>
-      <c r="J2102" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2102" t="inlineStr">
-        <is>
-          <t>odd-even-even-even-even-odd</t>
-        </is>
-      </c>
-      <c r="L2102" t="inlineStr">
-        <is>
-          <t>Even: 4, Odd: 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2103">
-      <c r="A2103" s="1" t="n">
-        <v>2101</v>
-      </c>
-      <c r="B2103" s="2" t="n">
-        <v>34773</v>
-      </c>
-      <c r="C2103" t="inlineStr">
-        <is>
-          <t>8,14,24,30,36,40</t>
-        </is>
-      </c>
-      <c r="D2103" t="n">
-        <v>8</v>
-      </c>
-      <c r="E2103" t="n">
-        <v>14</v>
-      </c>
-      <c r="F2103" t="n">
-        <v>24</v>
-      </c>
-      <c r="G2103" t="n">
-        <v>30</v>
-      </c>
-      <c r="H2103" t="n">
-        <v>36</v>
-      </c>
-      <c r="I2103" t="n">
-        <v>40</v>
-      </c>
-      <c r="J2103" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2103" t="inlineStr">
-        <is>
-          <t>even-even-even-even-even-even</t>
-        </is>
-      </c>
-      <c r="L2103" t="inlineStr">
-        <is>
-          <t>Even: 6, Odd: 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="2104">
-      <c r="A2104" s="1" t="n">
-        <v>2102</v>
-      </c>
-      <c r="B2104" s="2" t="n">
-        <v>34766</v>
-      </c>
-      <c r="C2104" t="inlineStr">
-        <is>
-          <t>4,20,22,30,34,38</t>
-        </is>
-      </c>
-      <c r="D2104" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2104" t="n">
-        <v>20</v>
-      </c>
-      <c r="F2104" t="n">
-        <v>22</v>
-      </c>
-      <c r="G2104" t="n">
-        <v>30</v>
-      </c>
-      <c r="H2104" t="n">
-        <v>34</v>
-      </c>
-      <c r="I2104" t="n">
-        <v>38</v>
-      </c>
-      <c r="J2104" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="K2104" t="inlineStr">
-        <is>
-          <t>even-even-even-even-even-even</t>
-        </is>
-      </c>
-      <c r="L2104" t="inlineStr">
-        <is>
-          <t>Even: 6, Odd: 0</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>